<commit_message>
adding ability to run on multiple browsers
</commit_message>
<xml_diff>
--- a/src/main/java/selenium_framework/test_cases/HyperTech_Automation_Test_Case.xlsx
+++ b/src/main/java/selenium_framework/test_cases/HyperTech_Automation_Test_Case.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nazmul.islam/Desktop/Personal/HyperTech/ht-selenium-framework/src/main/java/selenium_framework/test_cases/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DE55AF3-32D9-8347-A92B-79AED9A4F410}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F67CE054-203F-8347-8700-84F63F3BD141}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="72">
   <si>
     <t>TSID</t>
   </si>
@@ -64,15 +64,6 @@
   </si>
   <si>
     <t>Comments</t>
-  </si>
-  <si>
-    <t>Open a Browser</t>
-  </si>
-  <si>
-    <t>OpenBrowser</t>
-  </si>
-  <si>
-    <t>chrome</t>
   </si>
   <si>
     <t>Navigate http://hypertech.ai/contact.php</t>
@@ -145,9 +136,6 @@
   </si>
   <si>
     <t>Enter "Mobile" into the what field</t>
-  </si>
-  <si>
-    <t>//input[@id='mobile']</t>
   </si>
   <si>
     <t>Enter "Message" into the What field</t>
@@ -237,13 +225,28 @@
     <t>/api/process_contact.php</t>
   </si>
   <si>
-    <t xml:space="preserve">Close Browser </t>
+    <t>Passed</t>
   </si>
   <si>
-    <t>CloseBrowser</t>
+    <t>Failed</t>
   </si>
   <si>
-    <t>Passed</t>
+    <t>invalid selector: Unable to locate an element with the xpath expression //input[@id='mobile']1 because of the following error:
+SyntaxError: Failed to execute 'evaluate' on 'Document': The string '//input[@id='mobile']1' is not a valid XPath expression.
+  (Session info: chrome=88.0.4324.192)
+For documentation on this error, please visit: https://www.seleniumhq.org/exceptions/invalid_selector_exception.html
+Build info: version: '3.141.59', revision: 'e82be7d358', time: '2018-11-14T08:17:03'
+System info: host: 'LBURmacK1MXJGH8', ip: '192.168.1.145', os.name: 'Mac OS X', os.arch: 'x86_64', os.version: '10.16', java.version: '1.8.0_202'
+Driver info: org.openqa.selenium.chrome.ChromeDriver
+Capabilities {acceptInsecureCerts: false, browserName: chrome, browserVersion: 88.0.4324.192, chrome: {chromedriverVersion: 88.0.4324.96 (68dba2d8a0b14..., userDataDir: /var/folders/ys/ync08dys1ml...}, goog:chromeOptions: {debuggerAddress: localhost:55689}, javascriptEnabled: true, networkConnectionEnabled: false, pageLoadStrategy: normal, platform: MAC, platformName: MAC, proxy: Proxy(), setWindowRect: true, strictFileInteractability: false, timeouts: {implicit: 0, pageLoad: 300000, script: 30000}, unhandledPromptBehavior: dismiss and notify, webauthn:extension:largeBlob: true, webauthn:virtualAuthenticators: true}
+Session ID: ec3ec15e5f8002086a2ad1d419f1ae89
+*** Element info: {Using=xpath, value=//input[@id='mobile']1}</t>
+  </si>
+  <si>
+    <t>//input[@id='mobile']</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -669,10 +672,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z996"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -731,7 +734,7 @@
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1">
       <c r="A2" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>14</v>
@@ -741,7 +744,7 @@
       </c>
       <c r="D2" s="4"/>
       <c r="E2" s="4"/>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="8" t="s">
         <v>16</v>
       </c>
       <c r="G2" s="4"/>
@@ -767,43 +770,43 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1">
       <c r="A3" s="3">
-        <v>2</v>
+        <v>3</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="8" t="s">
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="4"/>
-      <c r="R3" s="4"/>
-      <c r="S3" s="4"/>
-      <c r="T3" s="4"/>
-      <c r="U3" s="4"/>
-      <c r="V3" s="4"/>
-      <c r="W3" s="4"/>
-      <c r="X3" s="4"/>
-      <c r="Y3" s="4"/>
-      <c r="Z3" s="4"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="12"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="12"/>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="12"/>
+      <c r="S3" s="12"/>
+      <c r="T3" s="12"/>
+      <c r="U3" s="12"/>
+      <c r="V3" s="12"/>
+      <c r="W3" s="12"/>
+      <c r="X3" s="12"/>
+      <c r="Y3" s="12"/>
+      <c r="Z3" s="12"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1">
       <c r="A4" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" s="9" t="s">
         <v>20</v>
@@ -813,9 +816,7 @@
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
-      <c r="F4" s="10" t="s">
-        <v>22</v>
-      </c>
+      <c r="F4" s="12"/>
       <c r="G4" s="12"/>
       <c r="H4" s="12"/>
       <c r="I4" s="12"/>
@@ -839,16 +840,20 @@
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1">
       <c r="A5" s="3">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B5" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="10" t="s">
+      <c r="D5" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
+      <c r="E5" s="10" t="s">
+        <v>25</v>
+      </c>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -873,16 +878,16 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1">
       <c r="A6" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E6" s="10" t="s">
         <v>28</v>
@@ -911,54 +916,60 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1">
       <c r="A7" s="3">
-        <v>6</v>
+        <v>7</v>
       </c>
-      <c r="B7" s="9" t="s">
+      <c r="B7" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="10" t="s">
+      <c r="C7" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D7" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="10" t="s">
+      <c r="D7" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="12"/>
-      <c r="I7" s="12"/>
-      <c r="J7" s="12"/>
-      <c r="K7" s="12"/>
-      <c r="L7" s="12"/>
-      <c r="M7" s="12"/>
-      <c r="N7" s="12"/>
-      <c r="O7" s="12"/>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="12"/>
-      <c r="R7" s="12"/>
-      <c r="S7" s="12"/>
-      <c r="T7" s="12"/>
-      <c r="U7" s="12"/>
-      <c r="V7" s="12"/>
-      <c r="W7" s="12"/>
-      <c r="X7" s="12"/>
-      <c r="Y7" s="12"/>
-      <c r="Z7" s="12"/>
+      <c r="E7" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="G7" t="s">
+        <v>67</v>
+      </c>
+      <c r="H7" t="s">
+        <v>71</v>
+      </c>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="4"/>
+      <c r="L7" s="4"/>
+      <c r="M7" s="4"/>
+      <c r="N7" s="4"/>
+      <c r="O7" s="4"/>
+      <c r="P7" s="4"/>
+      <c r="Q7" s="4"/>
+      <c r="R7" s="4"/>
+      <c r="S7" s="4"/>
+      <c r="T7" s="4"/>
+      <c r="U7" s="4"/>
+      <c r="V7" s="4"/>
+      <c r="W7" s="4"/>
+      <c r="X7" s="4"/>
+      <c r="Y7" s="4"/>
+      <c r="Z7" s="4"/>
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1">
       <c r="A8" s="3">
-        <v>7</v>
+        <v>8</v>
       </c>
-      <c r="B8" s="13" t="s">
-        <v>32</v>
+      <c r="B8" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>35</v>
@@ -967,9 +978,11 @@
         <v>36</v>
       </c>
       <c r="G8" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
-      <c r="H8" s="4"/>
+      <c r="H8" t="s">
+        <v>71</v>
+      </c>
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="4"/>
@@ -991,27 +1004,29 @@
     </row>
     <row r="9" spans="1:26" ht="15.75" customHeight="1">
       <c r="A9" s="3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>37</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
-      <c r="E9" s="4" t="s">
-        <v>38</v>
+      <c r="E9" s="10" t="s">
+        <v>70</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>39</v>
+      <c r="F9" s="3">
+        <v>5143005000</v>
       </c>
       <c r="G9" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
-      <c r="H9" s="4"/>
+      <c r="H9" t="s">
+        <v>71</v>
+      </c>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
@@ -1033,27 +1048,29 @@
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1">
       <c r="A10" s="3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>33</v>
+      <c r="G10" t="s">
+        <v>67</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>34</v>
+      <c r="H10" t="s">
+        <v>71</v>
       </c>
-      <c r="E10" s="10" t="s">
-        <v>41</v>
-      </c>
-      <c r="F10" s="3">
-        <v>5143005000</v>
-      </c>
-      <c r="G10" t="s">
-        <v>73</v>
-      </c>
-      <c r="H10" s="4"/>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
       <c r="K10" s="4"/>
@@ -1075,49 +1092,45 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1">
       <c r="A11" s="3">
-        <v>10</v>
+        <v>11</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="B11" s="14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E11" s="4" t="s">
+      <c r="D11" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="E11" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="G11" t="s">
-        <v>73</v>
-      </c>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
-      <c r="K11" s="4"/>
-      <c r="L11" s="4"/>
-      <c r="M11" s="4"/>
-      <c r="N11" s="4"/>
-      <c r="O11" s="4"/>
-      <c r="P11" s="4"/>
-      <c r="Q11" s="4"/>
-      <c r="R11" s="4"/>
-      <c r="S11" s="4"/>
-      <c r="T11" s="4"/>
-      <c r="U11" s="4"/>
-      <c r="V11" s="4"/>
-      <c r="W11" s="4"/>
-      <c r="X11" s="4"/>
-      <c r="Y11" s="4"/>
-      <c r="Z11" s="4"/>
+      <c r="F11" s="15"/>
+      <c r="G11" s="15"/>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="15"/>
+      <c r="O11" s="15"/>
+      <c r="P11" s="15"/>
+      <c r="Q11" s="15"/>
+      <c r="R11" s="15"/>
+      <c r="S11" s="15"/>
+      <c r="T11" s="15"/>
+      <c r="U11" s="15"/>
+      <c r="V11" s="15"/>
+      <c r="W11" s="15"/>
+      <c r="X11" s="15"/>
+      <c r="Y11" s="15"/>
+      <c r="Z11" s="15"/>
     </row>
     <row r="12" spans="1:26" ht="15.75" customHeight="1">
       <c r="A12" s="3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>45</v>
@@ -1125,13 +1138,15 @@
       <c r="C12" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="10" t="s">
+      <c r="D12" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="E12" s="14" t="s">
+      <c r="F12" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="F12" s="15"/>
       <c r="G12" s="15"/>
       <c r="H12" s="15"/>
       <c r="I12" s="15"/>
@@ -1155,7 +1170,7 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1">
       <c r="A13" s="3">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B13" s="14" t="s">
         <v>49</v>
@@ -1164,13 +1179,13 @@
         <v>50</v>
       </c>
       <c r="D13" s="14" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
-      <c r="F13" s="14" t="s">
-        <v>52</v>
+      <c r="F13" s="14">
+        <v>1</v>
       </c>
       <c r="G13" s="15"/>
       <c r="H13" s="15"/>
@@ -1195,23 +1210,21 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1">
       <c r="A14" s="3">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B14" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>52</v>
+      </c>
+      <c r="D14" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="E14" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="F14" s="14">
-        <v>1</v>
-      </c>
+      <c r="F14" s="15"/>
       <c r="G14" s="15"/>
       <c r="H14" s="15"/>
       <c r="I14" s="15"/>
@@ -1235,7 +1248,7 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1">
       <c r="A15" s="3">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B15" s="14" t="s">
         <v>55</v>
@@ -1244,10 +1257,10 @@
         <v>56</v>
       </c>
       <c r="D15" s="14" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E15" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F15" s="15"/>
       <c r="G15" s="15"/>
@@ -1273,59 +1286,61 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1">
       <c r="A16" s="3">
-        <v>15</v>
+        <v>16</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>43</v>
+      </c>
+      <c r="E16" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="C16" s="14" t="s">
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="4"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="4"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="4"/>
+      <c r="R16" s="4"/>
+      <c r="S16" s="4"/>
+      <c r="T16" s="4"/>
+      <c r="U16" s="4"/>
+      <c r="V16" s="4"/>
+      <c r="W16" s="4"/>
+      <c r="X16" s="4"/>
+      <c r="Y16" s="4"/>
+      <c r="Z16" s="4"/>
+    </row>
+    <row r="17" spans="1:26" ht="15.75" customHeight="1">
+      <c r="A17" s="3">
+        <v>17</v>
+      </c>
+      <c r="B17" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D16" s="14" t="s">
-        <v>57</v>
-      </c>
-      <c r="E16" s="14" t="s">
+      <c r="C17" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="15"/>
-      <c r="I16" s="15"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="15"/>
-      <c r="N16" s="15"/>
-      <c r="O16" s="15"/>
-      <c r="P16" s="15"/>
-      <c r="Q16" s="15"/>
-      <c r="R16" s="15"/>
-      <c r="S16" s="15"/>
-      <c r="T16" s="15"/>
-      <c r="U16" s="15"/>
-      <c r="V16" s="15"/>
-      <c r="W16" s="15"/>
-      <c r="X16" s="15"/>
-      <c r="Y16" s="15"/>
-      <c r="Z16" s="15"/>
-    </row>
-    <row r="17" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A17" s="3">
-        <v>16</v>
+      <c r="D17" s="10" t="s">
+        <v>43</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="E17" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="C17" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="D17" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E17" s="4" t="s">
+      <c r="F17" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
@@ -1349,113 +1364,95 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1">
       <c r="A18" s="3">
-        <v>17</v>
+        <v>18</v>
       </c>
-      <c r="B18" s="4" t="s">
+      <c r="B18" s="10" t="s">
         <v>64</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="10" t="s">
         <v>65</v>
       </c>
-      <c r="D18" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E18" s="10" t="s">
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="F18" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="G18" s="4"/>
-      <c r="H18" s="4"/>
-      <c r="I18" s="4"/>
-      <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="4"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="4"/>
-      <c r="O18" s="4"/>
-      <c r="P18" s="4"/>
-      <c r="Q18" s="4"/>
-      <c r="R18" s="4"/>
-      <c r="S18" s="4"/>
-      <c r="T18" s="4"/>
-      <c r="U18" s="4"/>
-      <c r="V18" s="4"/>
-      <c r="W18" s="4"/>
-      <c r="X18" s="4"/>
-      <c r="Y18" s="4"/>
-      <c r="Z18" s="4"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="12"/>
+      <c r="I18" s="12"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="12"/>
+      <c r="L18" s="12"/>
+      <c r="M18" s="12"/>
+      <c r="N18" s="12"/>
+      <c r="O18" s="12"/>
+      <c r="P18" s="12"/>
+      <c r="Q18" s="12"/>
+      <c r="R18" s="12"/>
+      <c r="S18" s="12"/>
+      <c r="T18" s="12"/>
+      <c r="U18" s="12"/>
+      <c r="V18" s="12"/>
+      <c r="W18" s="12"/>
+      <c r="X18" s="12"/>
+      <c r="Y18" s="12"/>
+      <c r="Z18" s="12"/>
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A19" s="3">
-        <v>18</v>
-      </c>
-      <c r="B19" s="10" t="s">
-        <v>68</v>
-      </c>
-      <c r="C19" s="10" t="s">
-        <v>69</v>
-      </c>
-      <c r="D19" s="12"/>
-      <c r="E19" s="12"/>
-      <c r="F19" s="10" t="s">
-        <v>70</v>
-      </c>
-      <c r="G19" s="12"/>
-      <c r="H19" s="12"/>
-      <c r="I19" s="12"/>
-      <c r="J19" s="12"/>
-      <c r="K19" s="12"/>
-      <c r="L19" s="12"/>
-      <c r="M19" s="12"/>
-      <c r="N19" s="12"/>
-      <c r="O19" s="12"/>
-      <c r="P19" s="12"/>
-      <c r="Q19" s="12"/>
-      <c r="R19" s="12"/>
-      <c r="S19" s="12"/>
-      <c r="T19" s="12"/>
-      <c r="U19" s="12"/>
-      <c r="V19" s="12"/>
-      <c r="W19" s="12"/>
-      <c r="X19" s="12"/>
-      <c r="Y19" s="12"/>
-      <c r="Z19" s="12"/>
+      <c r="A19" s="15"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="15"/>
+      <c r="D19" s="15"/>
+      <c r="E19" s="15"/>
+      <c r="F19" s="15"/>
+      <c r="G19" s="15"/>
+      <c r="H19" s="15"/>
+      <c r="I19" s="15"/>
+      <c r="J19" s="15"/>
+      <c r="K19" s="15"/>
+      <c r="L19" s="15"/>
+      <c r="M19" s="15"/>
+      <c r="N19" s="15"/>
+      <c r="O19" s="15"/>
+      <c r="P19" s="15"/>
+      <c r="Q19" s="15"/>
+      <c r="R19" s="15"/>
+      <c r="S19" s="15"/>
+      <c r="T19" s="15"/>
+      <c r="U19" s="15"/>
+      <c r="V19" s="15"/>
+      <c r="W19" s="15"/>
+      <c r="X19" s="15"/>
+      <c r="Y19" s="15"/>
+      <c r="Z19" s="15"/>
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1">
-      <c r="A20" s="3">
-        <v>19</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>71</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-      <c r="O20" s="4"/>
-      <c r="P20" s="4"/>
-      <c r="Q20" s="4"/>
-      <c r="R20" s="4"/>
-      <c r="S20" s="4"/>
-      <c r="T20" s="4"/>
-      <c r="U20" s="4"/>
-      <c r="V20" s="4"/>
-      <c r="W20" s="4"/>
-      <c r="X20" s="4"/>
-      <c r="Y20" s="4"/>
-      <c r="Z20" s="4"/>
+      <c r="A20" s="15"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="15"/>
+      <c r="E20" s="15"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="15"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="15"/>
+      <c r="P20" s="15"/>
+      <c r="Q20" s="15"/>
+      <c r="R20" s="15"/>
+      <c r="S20" s="15"/>
+      <c r="T20" s="15"/>
+      <c r="U20" s="15"/>
+      <c r="V20" s="15"/>
+      <c r="W20" s="15"/>
+      <c r="X20" s="15"/>
+      <c r="Y20" s="15"/>
+      <c r="Z20" s="15"/>
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1">
       <c r="A21" s="15"/>
@@ -2157,7 +2154,7 @@
       <c r="Y45" s="15"/>
       <c r="Z45" s="15"/>
     </row>
-    <row r="46" spans="1:26" ht="15.75" customHeight="1">
+    <row r="46" spans="1:26" ht="13">
       <c r="A46" s="15"/>
       <c r="B46" s="15"/>
       <c r="C46" s="15"/>
@@ -2185,7 +2182,7 @@
       <c r="Y46" s="15"/>
       <c r="Z46" s="15"/>
     </row>
-    <row r="47" spans="1:26" ht="15.75" customHeight="1">
+    <row r="47" spans="1:26" ht="13">
       <c r="A47" s="15"/>
       <c r="B47" s="15"/>
       <c r="C47" s="15"/>
@@ -28785,65 +28782,9 @@
       <c r="Y996" s="15"/>
       <c r="Z996" s="15"/>
     </row>
-    <row r="997" spans="1:26" ht="13">
-      <c r="A997" s="15"/>
-      <c r="B997" s="15"/>
-      <c r="C997" s="15"/>
-      <c r="D997" s="15"/>
-      <c r="E997" s="15"/>
-      <c r="F997" s="15"/>
-      <c r="G997" s="15"/>
-      <c r="H997" s="15"/>
-      <c r="I997" s="15"/>
-      <c r="J997" s="15"/>
-      <c r="K997" s="15"/>
-      <c r="L997" s="15"/>
-      <c r="M997" s="15"/>
-      <c r="N997" s="15"/>
-      <c r="O997" s="15"/>
-      <c r="P997" s="15"/>
-      <c r="Q997" s="15"/>
-      <c r="R997" s="15"/>
-      <c r="S997" s="15"/>
-      <c r="T997" s="15"/>
-      <c r="U997" s="15"/>
-      <c r="V997" s="15"/>
-      <c r="W997" s="15"/>
-      <c r="X997" s="15"/>
-      <c r="Y997" s="15"/>
-      <c r="Z997" s="15"/>
-    </row>
-    <row r="998" spans="1:26" ht="13">
-      <c r="A998" s="15"/>
-      <c r="B998" s="15"/>
-      <c r="C998" s="15"/>
-      <c r="D998" s="15"/>
-      <c r="E998" s="15"/>
-      <c r="F998" s="15"/>
-      <c r="G998" s="15"/>
-      <c r="H998" s="15"/>
-      <c r="I998" s="15"/>
-      <c r="J998" s="15"/>
-      <c r="K998" s="15"/>
-      <c r="L998" s="15"/>
-      <c r="M998" s="15"/>
-      <c r="N998" s="15"/>
-      <c r="O998" s="15"/>
-      <c r="P998" s="15"/>
-      <c r="Q998" s="15"/>
-      <c r="R998" s="15"/>
-      <c r="S998" s="15"/>
-      <c r="T998" s="15"/>
-      <c r="U998" s="15"/>
-      <c r="V998" s="15"/>
-      <c r="W998" s="15"/>
-      <c r="X998" s="15"/>
-      <c r="Y998" s="15"/>
-      <c r="Z998" s="15"/>
-    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F3" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>